<commit_message>
added Companies test scripts
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonia\Desktop\Crate\Crate\Crate\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonia\Desktop\CRATE\Crate\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="216">
   <si>
     <t>Username</t>
   </si>
@@ -564,21 +564,9 @@
     <t>.//*[@id='update-company-logo']</t>
   </si>
   <si>
-    <t>Xpath</t>
-  </si>
-  <si>
-    <t>//*[@id="top-bar-menu"]/div[1]/ul/li[6]/ul/li/a</t>
-  </si>
-  <si>
-    <t>//*[@id="top-bar-menu"]/div[1]/ul/li[6]/ul/li/ul/li[3]/a</t>
-  </si>
-  <si>
     <t xml:space="preserve">Companies </t>
   </si>
   <si>
-    <t>//a[@href='/Account/AddNewCompany']</t>
-  </si>
-  <si>
     <t>Add new</t>
   </si>
   <si>
@@ -618,9 +606,6 @@
     <t>.//*[@id='imgUpload']</t>
   </si>
   <si>
-    <t>.//*[@id='submitBtn']</t>
-  </si>
-  <si>
     <t>city</t>
   </si>
   <si>
@@ -639,18 +624,12 @@
     <t>email id</t>
   </si>
   <si>
-    <t>newsexport</t>
-  </si>
-  <si>
     <t>newsexport@gmail.com</t>
   </si>
   <si>
     <t>98 carlton gore rd, newmarket</t>
   </si>
   <si>
-    <t>Carlton</t>
-  </si>
-  <si>
     <t>//div[@class='pac-item'][1]</t>
   </si>
   <si>
@@ -658,6 +637,39 @@
   </si>
   <si>
     <t>http://experieco.com/</t>
+  </si>
+  <si>
+    <t>.//*[@id='top-bar-menu']/div[1]/ul/li[6]/ul/li/ul/li[3]/a</t>
+  </si>
+  <si>
+    <t>.//a[@href='/Account/AddNewCompany']</t>
+  </si>
+  <si>
+    <t>Carlton gore rd</t>
+  </si>
+  <si>
+    <t>Newmarket</t>
+  </si>
+  <si>
+    <t>Auckland</t>
+  </si>
+  <si>
+    <t>Newsexport</t>
+  </si>
+  <si>
+    <t>.//*[@id='btn4']</t>
+  </si>
+  <si>
+    <t>lastpage btn</t>
+  </si>
+  <si>
+    <t>alert</t>
+  </si>
+  <si>
+    <t>submitBtn</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -1608,10 +1620,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,21 +2196,24 @@
         <v>179</v>
       </c>
     </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" display="characters@"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2226,96 +2241,96 @@
         <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
         <v>59</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B7" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
         <v>65</v>
       </c>
       <c r="D7" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B9" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D9">
         <v>98</v>
@@ -2323,85 +2338,116 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B10" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>192</v>
+        <v>188</v>
+      </c>
+      <c r="D11" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B12" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>194</v>
+        <v>190</v>
+      </c>
+      <c r="D12" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B13" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>195</v>
+        <v>191</v>
+      </c>
+      <c r="D13">
+        <v>1023</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B14" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D14" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B15" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B16" t="s">
-        <v>180</v>
+        <v>215</v>
       </c>
       <c r="C16" t="s">
-        <v>198</v>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>213</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2409,5 +2455,6 @@
     <hyperlink ref="D6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>